<commit_message>
Upload Y3_B2526_GIT_&_Liver_reference_data.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/reference_data/Y3_B2526_GIT_&_Liver_reference_data.xlsx
+++ b/reference_data/Y3_B2526_GIT_&_Liver_reference_data.xlsx
@@ -479,7 +479,7 @@
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
-    <col width="46" customWidth="1" min="5" max="5"/>
+    <col width="42" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="E127" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7633,7 +7633,7 @@
       </c>
       <c r="E265" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9631,7 +9631,7 @@
       </c>
       <c r="E339" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9658,7 +9658,7 @@
       </c>
       <c r="E340" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="E342" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -10225,7 +10225,7 @@
       </c>
       <c r="E361" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="E378" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -13114,7 +13114,7 @@
       </c>
       <c r="E468" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -14356,7 +14356,7 @@
       </c>
       <c r="E514" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -14626,7 +14626,7 @@
       </c>
       <c r="E524" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -14896,7 +14896,7 @@
       </c>
       <c r="E534" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -14950,7 +14950,7 @@
       </c>
       <c r="E536" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -15328,7 +15328,7 @@
       </c>
       <c r="E550" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -15895,7 +15895,7 @@
       </c>
       <c r="E571" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16030,7 +16030,7 @@
       </c>
       <c r="E576" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16165,7 +16165,7 @@
       </c>
       <c r="E581" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16597,7 +16597,7 @@
       </c>
       <c r="E597" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16678,7 +16678,7 @@
       </c>
       <c r="E600" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16786,7 +16786,7 @@
       </c>
       <c r="E604" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16894,7 +16894,7 @@
       </c>
       <c r="E608" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -16948,7 +16948,7 @@
       </c>
       <c r="E610" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -17083,7 +17083,7 @@
       </c>
       <c r="E615" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -17812,7 +17812,7 @@
       </c>
       <c r="E642" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="E651" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -18136,7 +18136,7 @@
       </c>
       <c r="E654" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -18622,7 +18622,7 @@
       </c>
       <c r="E672" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -19162,7 +19162,7 @@
       </c>
       <c r="E692" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -20053,7 +20053,7 @@
       </c>
       <c r="E725" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -20269,7 +20269,7 @@
       </c>
       <c r="E733" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -20890,7 +20890,7 @@
       </c>
       <c r="E756" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -20917,7 +20917,7 @@
       </c>
       <c r="E757" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -21511,7 +21511,7 @@
       </c>
       <c r="E779" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -21970,7 +21970,7 @@
       </c>
       <c r="E796" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -21997,7 +21997,7 @@
       </c>
       <c r="E797" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -22294,7 +22294,7 @@
       </c>
       <c r="E808" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -22645,7 +22645,7 @@
       </c>
       <c r="E821" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -22915,7 +22915,7 @@
       </c>
       <c r="E831" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -23158,7 +23158,7 @@
       </c>
       <c r="E840" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -23914,7 +23914,7 @@
       </c>
       <c r="E868" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -23995,7 +23995,7 @@
       </c>
       <c r="E871" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -24346,7 +24346,7 @@
       </c>
       <c r="E884" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -24427,7 +24427,7 @@
       </c>
       <c r="E887" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -24832,7 +24832,7 @@
       </c>
       <c r="E902" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -25345,7 +25345,7 @@
       </c>
       <c r="E921" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -25561,7 +25561,7 @@
       </c>
       <c r="E929" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -25804,7 +25804,7 @@
       </c>
       <c r="E938" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -25939,7 +25939,7 @@
       </c>
       <c r="E943" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -25966,7 +25966,7 @@
       </c>
       <c r="E944" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -26155,7 +26155,7 @@
       </c>
       <c r="E951" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -26209,7 +26209,7 @@
       </c>
       <c r="E953" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -26263,7 +26263,7 @@
       </c>
       <c r="E955" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -26479,7 +26479,7 @@
       </c>
       <c r="E963" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -27559,7 +27559,7 @@
       </c>
       <c r="E1003" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -27613,7 +27613,7 @@
       </c>
       <c r="E1005" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -27964,7 +27964,7 @@
       </c>
       <c r="E1018" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -28369,7 +28369,7 @@
       </c>
       <c r="E1033" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -28585,7 +28585,7 @@
       </c>
       <c r="E1041" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -29692,7 +29692,7 @@
       </c>
       <c r="E1082" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -29908,7 +29908,7 @@
       </c>
       <c r="E1090" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -30583,7 +30583,7 @@
       </c>
       <c r="E1115" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -31042,7 +31042,7 @@
       </c>
       <c r="E1132" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -31258,7 +31258,7 @@
       </c>
       <c r="E1140" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -32014,7 +32014,7 @@
       </c>
       <c r="E1168" s="3" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -32365,7 +32365,7 @@
       </c>
       <c r="E1181" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -32527,7 +32527,7 @@
       </c>
       <c r="E1187" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -32581,7 +32581,7 @@
       </c>
       <c r="E1189" s="4" t="inlineStr">
         <is>
-          <t>Y3_B2526_GIT_&amp;_Liver_reference_data OLD.xlsx</t>
+          <t>Y3_B2526_GIT_&amp;_Liver_reference_data.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>